<commit_message>
Dailyweek and Weekly Report 15.02.2025 LeKhanhDuc
</commit_message>
<xml_diff>
--- a/Report/Project Weekly Report_LeKhanhDuc.xlsx
+++ b/Report/Project Weekly Report_LeKhanhDuc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRN222\ProjectFinal\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E030E1-5177-480B-A418-28B4FCAF9C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A400AFBE-D9B7-4279-8153-8B5438E1DD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>PROJECT REPORT</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>Support API documentation management and testing</t>
+  </si>
+  <si>
+    <t>Implement authentication &amp; authorization for backend security.</t>
+  </si>
+  <si>
+    <t>Implement authentication &amp; authorization in ASP.NET Core. Focus on security best practices, token-based authentication (JWT), and role-based access control (RBAC) to ensure secure API access</t>
   </si>
 </sst>
 </file>
@@ -479,7 +485,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -985,12 +991,20 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+    <row r="16" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>

</xml_diff>

<commit_message>
Dailyweek and Weekly Report 02.03.2025 LeKhanhDuc
</commit_message>
<xml_diff>
--- a/Report/Project Weekly Report_LeKhanhDuc.xlsx
+++ b/Report/Project Weekly Report_LeKhanhDuc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRN222\ProjectFinal\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A400AFBE-D9B7-4279-8153-8B5438E1DD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D8C4E6-39BA-43EB-A1F9-7044E3C25E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>PROJECT REPORT</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Implement authentication &amp; authorization in ASP.NET Core. Focus on security best practices, token-based authentication (JWT), and role-based access control (RBAC) to ensure secure API access</t>
+  </si>
+  <si>
+    <t>Home page, login, register, profile design</t>
+  </si>
+  <si>
+    <t>Design frontend application</t>
   </si>
 </sst>
 </file>
@@ -483,9 +489,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1169,10 +1175,18 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="B21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="11">
+        <v>45718</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>

</xml_diff>

<commit_message>
LeKhanhDuc DailyReport and Weekly report 21.03.2025
</commit_message>
<xml_diff>
--- a/Report/Project Weekly Report_LeKhanhDuc.xlsx
+++ b/Report/Project Weekly Report_LeKhanhDuc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRN222\ProjectPRN222\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C0DFE8-56B6-413A-8DBD-BCFC6491F468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463ACE89-6746-455D-A8CA-408B3125C43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>PROJECT REPORT</t>
   </si>
@@ -176,6 +176,12 @@
   <si>
     <t>Code backend and intergration frontend (Post, Ads, Contact)</t>
   </si>
+  <si>
+    <t>Create, Update, Delete Review</t>
+  </si>
+  <si>
+    <t>Code backend and commutication with frontend</t>
+  </si>
 </sst>
 </file>
 
@@ -265,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -284,6 +290,7 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -503,7 +510,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1295,10 +1302,18 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="12">
+        <v>45737</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>

</xml_diff>